<commit_message>
upload the notebook with a preliminary run with energy
</commit_message>
<xml_diff>
--- a/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ce_calibrated.xlsx
+++ b/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ce_calibrated.xlsx
@@ -20682,7 +20682,7 @@
         <v>173</v>
       </c>
       <c r="C107">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H107">
         <v>1</v>
@@ -20867,7 +20867,7 @@
         <v>174</v>
       </c>
       <c r="C108">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -21052,7 +21052,7 @@
         <v>175</v>
       </c>
       <c r="C109">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -21237,7 +21237,7 @@
         <v>176</v>
       </c>
       <c r="C110">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -21422,7 +21422,7 @@
         <v>177</v>
       </c>
       <c r="C111">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H111">
         <v>1</v>
@@ -21607,7 +21607,7 @@
         <v>178</v>
       </c>
       <c r="C112">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -21792,7 +21792,7 @@
         <v>179</v>
       </c>
       <c r="C113">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H113">
         <v>1</v>
@@ -21977,7 +21977,7 @@
         <v>180</v>
       </c>
       <c r="C114">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H114">
         <v>1</v>
@@ -22162,7 +22162,7 @@
         <v>181</v>
       </c>
       <c r="C115">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H115">
         <v>1</v>
@@ -22347,7 +22347,7 @@
         <v>182</v>
       </c>
       <c r="C116">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H116">
         <v>1</v>
@@ -22532,7 +22532,7 @@
         <v>183</v>
       </c>
       <c r="C117">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H117">
         <v>1</v>
@@ -22717,7 +22717,7 @@
         <v>184</v>
       </c>
       <c r="C118">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H118">
         <v>1</v>
@@ -22902,7 +22902,7 @@
         <v>185</v>
       </c>
       <c r="C119">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H119">
         <v>1</v>
@@ -23087,7 +23087,7 @@
         <v>186</v>
       </c>
       <c r="C120">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H120">
         <v>1</v>
@@ -23272,7 +23272,7 @@
         <v>187</v>
       </c>
       <c r="C121">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H121">
         <v>1</v>
@@ -23457,7 +23457,7 @@
         <v>188</v>
       </c>
       <c r="C122">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H122">
         <v>1</v>
@@ -23642,7 +23642,7 @@
         <v>189</v>
       </c>
       <c r="C123">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H123">
         <v>1</v>
@@ -23827,7 +23827,7 @@
         <v>190</v>
       </c>
       <c r="C124">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -24012,7 +24012,7 @@
         <v>191</v>
       </c>
       <c r="C125">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -24197,7 +24197,7 @@
         <v>192</v>
       </c>
       <c r="C126">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H126">
         <v>1</v>
@@ -24382,7 +24382,7 @@
         <v>193</v>
       </c>
       <c r="C127">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H127">
         <v>1</v>
@@ -24567,7 +24567,7 @@
         <v>194</v>
       </c>
       <c r="C128">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H128">
         <v>1</v>
@@ -24752,7 +24752,7 @@
         <v>195</v>
       </c>
       <c r="C129">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H129">
         <v>1</v>
@@ -24937,7 +24937,7 @@
         <v>196</v>
       </c>
       <c r="C130">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H130">
         <v>1</v>
@@ -25122,7 +25122,7 @@
         <v>197</v>
       </c>
       <c r="C131">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -25307,7 +25307,7 @@
         <v>198</v>
       </c>
       <c r="C132">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H132">
         <v>1</v>

</xml_diff>

<commit_message>
preliminary run with new data finished
</commit_message>
<xml_diff>
--- a/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ce_calibrated.xlsx
+++ b/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ce_calibrated.xlsx
@@ -20684,7 +20684,7 @@
         <v>173</v>
       </c>
       <c r="C107">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H107">
         <v>1</v>
@@ -20869,7 +20869,7 @@
         <v>174</v>
       </c>
       <c r="C108">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -21054,7 +21054,7 @@
         <v>175</v>
       </c>
       <c r="C109">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -21239,7 +21239,7 @@
         <v>176</v>
       </c>
       <c r="C110">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -21424,7 +21424,7 @@
         <v>177</v>
       </c>
       <c r="C111">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H111">
         <v>1</v>
@@ -21609,7 +21609,7 @@
         <v>178</v>
       </c>
       <c r="C112">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -21794,7 +21794,7 @@
         <v>179</v>
       </c>
       <c r="C113">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H113">
         <v>1</v>
@@ -21979,7 +21979,7 @@
         <v>180</v>
       </c>
       <c r="C114">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H114">
         <v>1</v>
@@ -22164,7 +22164,7 @@
         <v>181</v>
       </c>
       <c r="C115">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H115">
         <v>1</v>
@@ -22349,7 +22349,7 @@
         <v>182</v>
       </c>
       <c r="C116">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H116">
         <v>1</v>
@@ -22534,7 +22534,7 @@
         <v>183</v>
       </c>
       <c r="C117">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H117">
         <v>1</v>
@@ -22719,7 +22719,7 @@
         <v>184</v>
       </c>
       <c r="C118">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H118">
         <v>1</v>
@@ -22904,7 +22904,7 @@
         <v>185</v>
       </c>
       <c r="C119">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H119">
         <v>1</v>
@@ -23089,7 +23089,7 @@
         <v>186</v>
       </c>
       <c r="C120">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H120">
         <v>1</v>
@@ -23274,7 +23274,7 @@
         <v>187</v>
       </c>
       <c r="C121">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H121">
         <v>1</v>
@@ -23459,7 +23459,7 @@
         <v>188</v>
       </c>
       <c r="C122">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H122">
         <v>1</v>
@@ -23644,7 +23644,7 @@
         <v>189</v>
       </c>
       <c r="C123">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H123">
         <v>1</v>
@@ -23829,7 +23829,7 @@
         <v>190</v>
       </c>
       <c r="C124">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -24014,7 +24014,7 @@
         <v>191</v>
       </c>
       <c r="C125">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -24199,7 +24199,7 @@
         <v>192</v>
       </c>
       <c r="C126">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H126">
         <v>1</v>
@@ -24384,7 +24384,7 @@
         <v>193</v>
       </c>
       <c r="C127">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H127">
         <v>1</v>
@@ -24569,7 +24569,7 @@
         <v>194</v>
       </c>
       <c r="C128">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H128">
         <v>1</v>
@@ -24754,7 +24754,7 @@
         <v>195</v>
       </c>
       <c r="C129">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H129">
         <v>1</v>
@@ -24939,7 +24939,7 @@
         <v>196</v>
       </c>
       <c r="C130">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H130">
         <v>1</v>
@@ -25124,7 +25124,7 @@
         <v>197</v>
       </c>
       <c r="C131">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -25309,7 +25309,7 @@
         <v>198</v>
       </c>
       <c r="C132">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H132">
         <v>1</v>

</xml_diff>